<commit_message>
corrected some upstream FTPC issues with new sampling frame column that was replaced in database - still need to do EIPS when databases are ready. corrected whitespace issue in sampling frame. Updated MapPACNVeg().
</commit_message>
<xml_diff>
--- a/R/PACN_veg_names.xlsx
+++ b/R/PACN_veg_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JJGross\Documents\RData\PROJECTS\pacnvegetation\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JJGross\Documents\R_projects\pacnvegetation\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F294B5C3-965C-4ED5-8C24-75A271599374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23512C3-76CF-466B-BE41-2B8ACFD0169A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="33120" yWindow="735" windowWidth="17010" windowHeight="17325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PACN_veg_names" sheetId="1" r:id="rId1"/>
@@ -208,9 +208,6 @@
     <t>Haleakalā</t>
   </si>
   <si>
-    <t> Puʻu Aliʻi </t>
-  </si>
-  <si>
     <t>Hoʻolehua</t>
   </si>
   <si>
@@ -251,12 +248,15 @@
   </si>
   <si>
     <t>Limestone Forest</t>
+  </si>
+  <si>
+    <t>Puʻu Aliʻi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1090,11 +1090,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1123,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1135,7 +1135,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1143,16 +1143,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1172,16 +1172,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -1201,16 +1201,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -1230,16 +1230,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
@@ -1259,16 +1259,16 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -1280,7 +1280,7 @@
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1288,16 +1288,16 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -1317,16 +1317,16 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -1349,13 +1349,13 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
         <v>65</v>
       </c>
-      <c r="D9" t="s">
-        <v>66</v>
-      </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -1367,7 +1367,7 @@
         <v>32</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1378,13 +1378,13 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
         <v>65</v>
       </c>
-      <c r="D10" t="s">
-        <v>66</v>
-      </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -1407,13 +1407,13 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
         <v>65</v>
       </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -1425,7 +1425,7 @@
         <v>36</v>
       </c>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1442,7 +1442,7 @@
         <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -1468,10 +1468,10 @@
         <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -1483,7 +1483,7 @@
         <v>44</v>
       </c>
       <c r="I13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
         <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F14" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
many various fixes while checking rendered reports
</commit_message>
<xml_diff>
--- a/R/PACN_veg_names.xlsx
+++ b/R/PACN_veg_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JJGross\Documents\R_projects\pacnvegetation\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23512C3-76CF-466B-BE41-2B8ACFD0169A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0A8E9B-E927-4418-900D-56269E2229BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33120" yWindow="735" windowWidth="17010" windowHeight="17325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32055" yWindow="1365" windowWidth="21825" windowHeight="14925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PACN_veg_names" sheetId="1" r:id="rId1"/>
@@ -202,9 +202,6 @@
     <t>Nāhuku / East Rift </t>
   </si>
   <si>
-    <t>Kīpahulu District</t>
-  </si>
-  <si>
     <t>Haleakalā</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>Puʻu Aliʻi</t>
+  </si>
+  <si>
+    <t>Kīpahulu District</t>
   </si>
 </sst>
 </file>
@@ -795,9 +795,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -835,7 +835,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -941,7 +941,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1083,7 +1083,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1094,7 +1094,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1123,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1135,7 +1135,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1143,16 +1143,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1172,16 +1172,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -1201,16 +1201,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -1230,16 +1230,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
@@ -1259,16 +1259,16 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -1280,7 +1280,7 @@
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1288,16 +1288,16 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -1309,7 +1309,7 @@
         <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1317,16 +1317,16 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -1338,7 +1338,7 @@
         <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1349,13 +1349,13 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
         <v>64</v>
       </c>
-      <c r="D9" t="s">
-        <v>65</v>
-      </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -1367,7 +1367,7 @@
         <v>32</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1378,13 +1378,13 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
         <v>64</v>
       </c>
-      <c r="D10" t="s">
-        <v>65</v>
-      </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -1407,13 +1407,13 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
         <v>64</v>
       </c>
-      <c r="D11" t="s">
-        <v>65</v>
-      </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -1425,7 +1425,7 @@
         <v>36</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1442,7 +1442,7 @@
         <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -1468,10 +1468,10 @@
         <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -1483,7 +1483,7 @@
         <v>44</v>
       </c>
       <c r="I13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
         <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F14" t="s">
         <v>48</v>

</xml_diff>